<commit_message>
cap nhat quan 8
</commit_message>
<xml_diff>
--- a/data/khaosat.xlsx
+++ b/data/khaosat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cscctphcm-my.sharepoint.com/personal/gdcsbac_cscctphcm_onmicrosoft_com/Documents/webdemo/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="586" documentId="13_ncr:1_{2EDB2D67-B674-4A3F-BBBF-6356067A4A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E70C54A-2E68-4AB9-95D0-538C38B49038}"/>
+  <xr:revisionPtr revIDLastSave="589" documentId="13_ncr:1_{2EDB2D67-B674-4A3F-BBBF-6356067A4A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67146408-2BD9-48D3-B149-5938CB415E55}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1266DFF-32F5-4B0B-A729-2A44814C55C6}"/>
   </bookViews>
@@ -6343,8 +6343,8 @@
   <dimension ref="A1:P663"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A644" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J607" sqref="J607"/>
+      <pane ySplit="1" topLeftCell="A590" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K610" sqref="K610"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -23636,17 +23636,17 @@
       </c>
       <c r="C608" s="23" t="str">
         <f t="shared" ref="C608:C663" si="4">LEFT(E608,2)&amp;"."&amp;RIGHT(E608,LEN(E608)-2)</f>
-        <v>11.874629700</v>
+        <v>10.736547729</v>
       </c>
       <c r="D608" s="23" t="str">
         <f t="shared" ref="D608:D663" si="5">LEFT(F608,2)&amp;"."&amp;RIGHT(F608,LEN(F608)-2)</f>
-        <v>59.86733572</v>
+        <v>10.6653933643</v>
       </c>
       <c r="E608" s="4">
-        <v>11874629700</v>
+        <v>10736547729</v>
       </c>
       <c r="F608" s="4">
-        <v>5986733572</v>
+        <v>106653933643</v>
       </c>
       <c r="N608" s="1" t="s">
         <v>1655</v>
@@ -23658,17 +23658,17 @@
       </c>
       <c r="C609" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.874912681</v>
+        <v>10.736804021</v>
       </c>
       <c r="D609" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.86557565</v>
+        <v>10.6653773500</v>
       </c>
       <c r="E609" s="4">
-        <v>11874912681</v>
+        <v>10736804021</v>
       </c>
       <c r="F609" s="4">
-        <v>5986557565</v>
+        <v>106653773500</v>
       </c>
       <c r="N609" s="1" t="s">
         <v>1655</v>
@@ -23680,17 +23680,17 @@
       </c>
       <c r="C610" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.875265360</v>
+        <v>10.737123400</v>
       </c>
       <c r="D610" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.86351766</v>
+        <v>10.6653586309</v>
       </c>
       <c r="E610" s="4">
-        <v>11875265360</v>
+        <v>10737123400</v>
       </c>
       <c r="F610" s="4">
-        <v>5986351766</v>
+        <v>106653586309</v>
       </c>
       <c r="N610" s="1" t="s">
         <v>1655</v>
@@ -23702,17 +23702,17 @@
       </c>
       <c r="C611" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.875560744</v>
+        <v>10.737390755</v>
       </c>
       <c r="D611" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.86231800</v>
+        <v>10.6653477432</v>
       </c>
       <c r="E611" s="4">
-        <v>11875560744</v>
+        <v>10737390755</v>
       </c>
       <c r="F611" s="4">
-        <v>5986231800</v>
+        <v>106653477432</v>
       </c>
       <c r="N611" s="1" t="s">
         <v>1655</v>
@@ -23724,17 +23724,17 @@
       </c>
       <c r="C612" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.875904814</v>
+        <v>10.737701841</v>
       </c>
       <c r="D612" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.86218620</v>
+        <v>10.6653466308</v>
       </c>
       <c r="E612" s="4">
-        <v>11875904814</v>
+        <v>10737701841</v>
       </c>
       <c r="F612" s="4">
-        <v>5986218620</v>
+        <v>106653466308</v>
       </c>
       <c r="N612" s="1" t="s">
         <v>1655</v>
@@ -23746,17 +23746,17 @@
       </c>
       <c r="C613" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.876198416</v>
+        <v>10.737967314</v>
       </c>
       <c r="D613" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.86200202</v>
+        <v>10.6653450259</v>
       </c>
       <c r="E613" s="4">
-        <v>11876198416</v>
+        <v>10737967314</v>
       </c>
       <c r="F613" s="4">
-        <v>5986200202</v>
+        <v>106653450259</v>
       </c>
       <c r="N613" s="1" t="s">
         <v>1655</v>
@@ -23768,17 +23768,17 @@
       </c>
       <c r="C614" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.875169554</v>
+        <v>10.737036733</v>
       </c>
       <c r="D614" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.86372323</v>
+        <v>10.6653604844</v>
       </c>
       <c r="E614" s="4">
-        <v>11875169554</v>
+        <v>10737036733</v>
       </c>
       <c r="F614" s="4">
-        <v>5986372323</v>
+        <v>106653604844</v>
       </c>
       <c r="N614" s="1" t="s">
         <v>1655</v>
@@ -23790,17 +23790,17 @@
       </c>
       <c r="C615" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.875106436</v>
+        <v>10.736979884</v>
       </c>
       <c r="D615" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.86292966</v>
+        <v>10.6653532127</v>
       </c>
       <c r="E615" s="4">
-        <v>11875106436</v>
+        <v>10736979884</v>
       </c>
       <c r="F615" s="4">
-        <v>5986292966</v>
+        <v>106653532127</v>
       </c>
       <c r="N615" s="1" t="s">
         <v>1655</v>
@@ -23812,17 +23812,17 @@
       </c>
       <c r="C616" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.874460252</v>
+        <v>10.736395654</v>
       </c>
       <c r="D616" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.86315106</v>
+        <v>10.6653550629</v>
       </c>
       <c r="E616" s="4">
-        <v>11874460252</v>
+        <v>10736395654</v>
       </c>
       <c r="F616" s="4">
-        <v>5986315106</v>
+        <v>106653550629</v>
       </c>
       <c r="N616" s="1" t="s">
         <v>1655</v>
@@ -23834,17 +23834,17 @@
       </c>
       <c r="C617" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.874121765</v>
+        <v>10.736089608</v>
       </c>
       <c r="D617" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.86331277</v>
+        <v>10.6653564502</v>
       </c>
       <c r="E617" s="4">
-        <v>11874121765</v>
+        <v>10736089608</v>
       </c>
       <c r="F617" s="4">
-        <v>5986331277</v>
+        <v>106653564502</v>
       </c>
       <c r="N617" s="1" t="s">
         <v>1655</v>
@@ -23856,17 +23856,17 @@
       </c>
       <c r="C618" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.873967693</v>
+        <v>10.735950312</v>
       </c>
       <c r="D618" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.86335484</v>
+        <v>10.6653567934</v>
       </c>
       <c r="E618" s="4">
-        <v>11873967693</v>
+        <v>10735950312</v>
       </c>
       <c r="F618" s="4">
-        <v>5986335484</v>
+        <v>106653567934</v>
       </c>
       <c r="N618" s="1" t="s">
         <v>1655</v>
@@ -23878,17 +23878,17 @@
       </c>
       <c r="C619" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.873668346</v>
+        <v>10.735679599</v>
       </c>
       <c r="D619" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.86370460</v>
+        <v>10.6653599103</v>
       </c>
       <c r="E619" s="4">
-        <v>11873668346</v>
+        <v>10735679599</v>
       </c>
       <c r="F619" s="4">
-        <v>5986370460</v>
+        <v>106653599103</v>
       </c>
       <c r="N619" s="1" t="s">
         <v>1655</v>
@@ -23900,17 +23900,17 @@
       </c>
       <c r="C620" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.873548714</v>
+        <v>10.735571406</v>
       </c>
       <c r="D620" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.86386378</v>
+        <v>10.6653613333</v>
       </c>
       <c r="E620" s="4">
-        <v>11873548714</v>
+        <v>10735571406</v>
       </c>
       <c r="F620" s="4">
-        <v>5986386378</v>
+        <v>106653613333</v>
       </c>
       <c r="N620" s="1" t="s">
         <v>1655</v>
@@ -23922,17 +23922,17 @@
       </c>
       <c r="C621" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.873339517</v>
+        <v>10.735382214</v>
       </c>
       <c r="D621" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.86413412</v>
+        <v>10.6653637485</v>
       </c>
       <c r="E621" s="4">
-        <v>11873339517</v>
+        <v>10735382214</v>
       </c>
       <c r="F621" s="4">
-        <v>5986413412</v>
+        <v>106653637485</v>
       </c>
       <c r="N621" s="1" t="s">
         <v>1655</v>
@@ -23944,17 +23944,17 @@
       </c>
       <c r="C622" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.873138193</v>
+        <v>10.735200117</v>
       </c>
       <c r="D622" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.86448627</v>
+        <v>10.6653669136</v>
       </c>
       <c r="E622" s="4">
-        <v>11873138193</v>
+        <v>10735200117</v>
       </c>
       <c r="F622" s="4">
-        <v>5986448627</v>
+        <v>106653669136</v>
       </c>
       <c r="N622" s="1" t="s">
         <v>1655</v>
@@ -23966,17 +23966,17 @@
       </c>
       <c r="C623" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.873867526</v>
+        <v>10.735859999</v>
       </c>
       <c r="D623" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.86243232</v>
+        <v>10.6653483333</v>
       </c>
       <c r="E623" s="4">
-        <v>11873867526</v>
+        <v>10735859999</v>
       </c>
       <c r="F623" s="4">
-        <v>5986243232</v>
+        <v>106653483333</v>
       </c>
       <c r="N623" s="1" t="s">
         <v>1655</v>
@@ -23988,17 +23988,17 @@
       </c>
       <c r="C624" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.873951282</v>
+        <v>10.735936216</v>
       </c>
       <c r="D624" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.86056961</v>
+        <v>10.6653313266</v>
       </c>
       <c r="E624" s="4">
-        <v>11873951282</v>
+        <v>10735936216</v>
       </c>
       <c r="F624" s="4">
-        <v>5986056961</v>
+        <v>106653313266</v>
       </c>
       <c r="N624" s="1" t="s">
         <v>1655</v>
@@ -24010,17 +24010,17 @@
       </c>
       <c r="C625" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.873937601</v>
+        <v>10.735924439</v>
       </c>
       <c r="D625" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.85834210</v>
+        <v>10.6653109593</v>
       </c>
       <c r="E625" s="4">
-        <v>11873937601</v>
+        <v>10735924439</v>
       </c>
       <c r="F625" s="4">
-        <v>5985834210</v>
+        <v>106653109593</v>
       </c>
       <c r="N625" s="1" t="s">
         <v>1655</v>
@@ -24032,17 +24032,17 @@
       </c>
       <c r="C626" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.874362695</v>
+        <v>10.736308333</v>
       </c>
       <c r="D626" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.85986546</v>
+        <v>10.6653250000</v>
       </c>
       <c r="E626" s="4">
-        <v>11874362695</v>
+        <v>10736308333</v>
       </c>
       <c r="F626" s="4">
-        <v>5985986546</v>
+        <v>106653250000</v>
       </c>
       <c r="N626" s="1" t="s">
         <v>1655</v>
@@ -24054,17 +24054,17 @@
       </c>
       <c r="C627" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.874255818</v>
+        <v>10.736198173</v>
       </c>
       <c r="D627" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.91072354</v>
+        <v>10.6657899109</v>
       </c>
       <c r="E627" s="4">
-        <v>11874255818</v>
+        <v>10736198173</v>
       </c>
       <c r="F627" s="4">
-        <v>5991072354</v>
+        <v>106657899109</v>
       </c>
       <c r="N627" s="1" t="s">
         <v>1655</v>
@@ -24076,17 +24076,17 @@
       </c>
       <c r="C628" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.874248143</v>
+        <v>10.736191841</v>
       </c>
       <c r="D628" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.90844791</v>
+        <v>10.6657691051</v>
       </c>
       <c r="E628" s="4">
-        <v>11874248143</v>
+        <v>10736191841</v>
       </c>
       <c r="F628" s="4">
-        <v>5990844791</v>
+        <v>106657691051</v>
       </c>
       <c r="N628" s="1" t="s">
         <v>1655</v>
@@ -24098,17 +24098,17 @@
       </c>
       <c r="C629" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.874198346</v>
+        <v>10.736147375</v>
       </c>
       <c r="D629" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.90638050</v>
+        <v>10.6657501917</v>
       </c>
       <c r="E629" s="4">
-        <v>11874198346</v>
+        <v>10736147375</v>
       </c>
       <c r="F629" s="4">
-        <v>5990638050</v>
+        <v>106657501917</v>
       </c>
       <c r="N629" s="1" t="s">
         <v>1655</v>
@@ -24120,17 +24120,17 @@
       </c>
       <c r="C630" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.874192938</v>
+        <v>10.736143080</v>
       </c>
       <c r="D630" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.90415808</v>
+        <v>10.6657298731</v>
       </c>
       <c r="E630" s="4">
-        <v>11874192938</v>
+        <v>10736143080</v>
       </c>
       <c r="F630" s="4">
-        <v>5990415808</v>
+        <v>106657298731</v>
       </c>
       <c r="N630" s="1" t="s">
         <v>1655</v>
@@ -24142,17 +24142,17 @@
       </c>
       <c r="C631" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.874197081</v>
+        <v>10.736147385</v>
       </c>
       <c r="D631" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.90205785</v>
+        <v>10.6657106741</v>
       </c>
       <c r="E631" s="4">
-        <v>11874197081</v>
+        <v>10736147385</v>
       </c>
       <c r="F631" s="4">
-        <v>5990205785</v>
+        <v>106657106741</v>
       </c>
       <c r="N631" s="1" t="s">
         <v>1655</v>
@@ -24164,17 +24164,17 @@
       </c>
       <c r="C632" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.874222824</v>
+        <v>10.736171062</v>
       </c>
       <c r="D632" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.90054087</v>
+        <v>10.6656968129</v>
       </c>
       <c r="E632" s="4">
-        <v>11874222824</v>
+        <v>10736171062</v>
       </c>
       <c r="F632" s="4">
-        <v>5990054087</v>
+        <v>106656968129</v>
       </c>
       <c r="N632" s="1" t="s">
         <v>1655</v>
@@ -24186,17 +24186,17 @@
       </c>
       <c r="C633" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.874210084</v>
+        <v>10.736160120</v>
       </c>
       <c r="D633" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.89838481</v>
+        <v>10.6656770990</v>
       </c>
       <c r="E633" s="4">
-        <v>11874210084</v>
+        <v>10736160120</v>
       </c>
       <c r="F633" s="4">
-        <v>5989838481</v>
+        <v>106656770990</v>
       </c>
       <c r="N633" s="1" t="s">
         <v>1655</v>
@@ -24208,17 +24208,17 @@
       </c>
       <c r="C634" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.873917433</v>
+        <v>10.735892861</v>
       </c>
       <c r="D634" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.90848341</v>
+        <v>10.6657693403</v>
       </c>
       <c r="E634" s="4">
-        <v>11873917433</v>
+        <v>10735892861</v>
       </c>
       <c r="F634" s="4">
-        <v>5990848341</v>
+        <v>106657693403</v>
       </c>
       <c r="N634" s="1" t="s">
         <v>1655</v>
@@ -24230,17 +24230,17 @@
       </c>
       <c r="C635" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.873644511</v>
+        <v>10.735646134</v>
       </c>
       <c r="D635" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.90847179</v>
+        <v>10.6657691604</v>
       </c>
       <c r="E635" s="4">
-        <v>11873644511</v>
+        <v>10735646134</v>
       </c>
       <c r="F635" s="4">
-        <v>5990847179</v>
+        <v>106657691604</v>
       </c>
       <c r="N635" s="1" t="s">
         <v>1655</v>
@@ -24252,17 +24252,17 @@
       </c>
       <c r="C636" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.873404352</v>
+        <v>10.735428935</v>
       </c>
       <c r="D636" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.90880317</v>
+        <v>10.6657721250</v>
       </c>
       <c r="E636" s="4">
-        <v>11873404352</v>
+        <v>10735428935</v>
       </c>
       <c r="F636" s="4">
-        <v>5990880317</v>
+        <v>106657721250</v>
       </c>
       <c r="N636" s="1" t="s">
         <v>1655</v>
@@ -24274,17 +24274,17 @@
       </c>
       <c r="C637" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.873400176</v>
+        <v>10.735425966</v>
       </c>
       <c r="D637" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.90578155</v>
+        <v>10.6657445006</v>
       </c>
       <c r="E637" s="4">
-        <v>11873400176</v>
+        <v>10735425966</v>
       </c>
       <c r="F637" s="4">
-        <v>5990578155</v>
+        <v>106657445006</v>
       </c>
       <c r="N637" s="1" t="s">
         <v>1655</v>
@@ -24296,17 +24296,17 @@
       </c>
       <c r="C638" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.873348062</v>
+        <v>10.735379041</v>
       </c>
       <c r="D638" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.90507573</v>
+        <v>10.6657380339</v>
       </c>
       <c r="E638" s="4">
-        <v>11873348062</v>
+        <v>10735379041</v>
       </c>
       <c r="F638" s="4">
-        <v>5990507573</v>
+        <v>106657380339</v>
       </c>
       <c r="N638" s="1" t="s">
         <v>1655</v>
@@ -24318,17 +24318,17 @@
       </c>
       <c r="C639" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.873398712</v>
+        <v>10.735425379</v>
       </c>
       <c r="D639" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.90301838</v>
+        <v>10.6657192396</v>
       </c>
       <c r="E639" s="4">
-        <v>11873398712</v>
+        <v>10735425379</v>
       </c>
       <c r="F639" s="4">
-        <v>5990301838</v>
+        <v>106657192396</v>
       </c>
       <c r="N639" s="1" t="s">
         <v>1655</v>
@@ -24340,17 +24340,17 @@
       </c>
       <c r="C640" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.873416692</v>
+        <v>10.735441891</v>
       </c>
       <c r="D640" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.90205546</v>
+        <v>10.6657104415</v>
       </c>
       <c r="E640" s="4">
-        <v>11873416692</v>
+        <v>10735441891</v>
       </c>
       <c r="F640" s="4">
-        <v>5990205546</v>
+        <v>106657104415</v>
       </c>
       <c r="N640" s="1" t="s">
         <v>1655</v>
@@ -24362,17 +24362,17 @@
       </c>
       <c r="C641" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.873416919</v>
+        <v>10.735442347</v>
       </c>
       <c r="D641" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.90111360</v>
+        <v>10.6657018311</v>
       </c>
       <c r="E641" s="4">
-        <v>11873416919</v>
+        <v>10735442347</v>
       </c>
       <c r="F641" s="4">
-        <v>5990111360</v>
+        <v>106657018311</v>
       </c>
       <c r="N641" s="1" t="s">
         <v>1655</v>
@@ -24384,17 +24384,17 @@
       </c>
       <c r="C642" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.873391449</v>
+        <v>10.735420052</v>
       </c>
       <c r="D642" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.89837267</v>
+        <v>10.6656767670</v>
       </c>
       <c r="E642" s="4">
-        <v>11873391449</v>
+        <v>10735420052</v>
       </c>
       <c r="F642" s="4">
-        <v>5989837267</v>
+        <v>106656767670</v>
       </c>
       <c r="N642" s="1" t="s">
         <v>1655</v>
@@ -24406,17 +24406,17 @@
       </c>
       <c r="C643" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.873381870</v>
+        <v>10.735411917</v>
       </c>
       <c r="D643" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.89640874</v>
+        <v>10.6656588103</v>
       </c>
       <c r="E643" s="4">
-        <v>11873381870</v>
+        <v>10735411917</v>
       </c>
       <c r="F643" s="4">
-        <v>5989640874</v>
+        <v>106656588103</v>
       </c>
       <c r="N643" s="1" t="s">
         <v>1655</v>
@@ -24428,17 +24428,17 @@
       </c>
       <c r="C644" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.871088543</v>
+        <v>10.733340000</v>
       </c>
       <c r="D644" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.89144711</v>
+        <v>10.6656128333</v>
       </c>
       <c r="E644" s="4">
-        <v>11871088543</v>
+        <v>10733340000</v>
       </c>
       <c r="F644" s="4">
-        <v>5989144711</v>
+        <v>106656128333</v>
       </c>
       <c r="N644" s="1" t="s">
         <v>1655</v>
@@ -24450,17 +24450,17 @@
       </c>
       <c r="C645" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.873044838</v>
+        <v>10.735108333</v>
       </c>
       <c r="D645" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.89226449</v>
+        <v>10.6656208334</v>
       </c>
       <c r="E645" s="4">
-        <v>11873044838</v>
+        <v>10735108333</v>
       </c>
       <c r="F645" s="4">
-        <v>5989226449</v>
+        <v>106656208334</v>
       </c>
       <c r="N645" s="1" t="s">
         <v>1655</v>
@@ -24472,17 +24472,17 @@
       </c>
       <c r="C646" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.873044838</v>
+        <v>10.735108333</v>
       </c>
       <c r="D646" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.89226449</v>
+        <v>10.6656208334</v>
       </c>
       <c r="E646" s="4">
-        <v>11873044838</v>
+        <v>10735108333</v>
       </c>
       <c r="F646" s="4">
-        <v>5989226449</v>
+        <v>106656208334</v>
       </c>
       <c r="N646" s="1" t="s">
         <v>1655</v>
@@ -24494,17 +24494,17 @@
       </c>
       <c r="C647" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.870781970</v>
+        <v>10.733062585</v>
       </c>
       <c r="D647" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.89243968</v>
+        <v>10.6656218246</v>
       </c>
       <c r="E647" s="4">
-        <v>11870781970</v>
+        <v>10733062585</v>
       </c>
       <c r="F647" s="4">
-        <v>5989243968</v>
+        <v>106656218246</v>
       </c>
       <c r="N647" s="1" t="s">
         <v>1655</v>
@@ -24516,17 +24516,17 @@
       </c>
       <c r="C648" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.870797249</v>
+        <v>10.733075679</v>
       </c>
       <c r="D648" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.89513540</v>
+        <v>10.6656464724</v>
       </c>
       <c r="E648" s="4">
-        <v>11870797249</v>
+        <v>10733075679</v>
       </c>
       <c r="F648" s="4">
-        <v>5989513540</v>
+        <v>106656464724</v>
       </c>
       <c r="N648" s="1" t="s">
         <v>1655</v>
@@ -24538,17 +24538,17 @@
       </c>
       <c r="C649" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.870809541</v>
+        <v>10.733086270</v>
       </c>
       <c r="D649" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.89709095</v>
+        <v>10.6656643530</v>
       </c>
       <c r="E649" s="4">
-        <v>11870809541</v>
+        <v>10733086270</v>
       </c>
       <c r="F649" s="4">
-        <v>5989709095</v>
+        <v>106656643530</v>
       </c>
       <c r="N649" s="1" t="s">
         <v>1655</v>
@@ -24560,17 +24560,17 @@
       </c>
       <c r="C650" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.870826480</v>
+        <v>10.733100765</v>
       </c>
       <c r="D650" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.90016114</v>
+        <v>10.6656924248</v>
       </c>
       <c r="E650" s="4">
-        <v>11870826480</v>
+        <v>10733100765</v>
       </c>
       <c r="F650" s="4">
-        <v>5990016114</v>
+        <v>106656924248</v>
       </c>
       <c r="N650" s="1" t="s">
         <v>1655</v>
@@ -24582,17 +24582,17 @@
       </c>
       <c r="C651" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.870843907</v>
+        <v>10.733116314</v>
       </c>
       <c r="D651" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.90093334</v>
+        <v>10.6656994887</v>
       </c>
       <c r="E651" s="4">
-        <v>11870843907</v>
+        <v>10733116314</v>
       </c>
       <c r="F651" s="4">
-        <v>5990093334</v>
+        <v>106656994887</v>
       </c>
       <c r="N651" s="1" t="s">
         <v>1655</v>
@@ -24604,17 +24604,17 @@
       </c>
       <c r="C652" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.870826606</v>
+        <v>10.733100213</v>
       </c>
       <c r="D652" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.90265997</v>
+        <v>10.6657152686</v>
       </c>
       <c r="E652" s="4">
-        <v>11870826606</v>
+        <v>10733100213</v>
       </c>
       <c r="F652" s="4">
-        <v>5990265997</v>
+        <v>106657152686</v>
       </c>
       <c r="N652" s="1" t="s">
         <v>1655</v>
@@ -24626,17 +24626,17 @@
       </c>
       <c r="C653" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.870836447</v>
+        <v>10.733108626</v>
       </c>
       <c r="D653" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.90447299</v>
+        <v>10.6657318456</v>
       </c>
       <c r="E653" s="4">
-        <v>11870836447</v>
+        <v>10733108626</v>
       </c>
       <c r="F653" s="4">
-        <v>5990447299</v>
+        <v>106657318456</v>
       </c>
       <c r="N653" s="1" t="s">
         <v>1655</v>
@@ -24648,17 +24648,17 @@
       </c>
       <c r="C654" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.870647687</v>
+        <v>10.732938935</v>
       </c>
       <c r="D654" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.90089529</v>
+        <v>10.6656990879</v>
       </c>
       <c r="E654" s="4">
-        <v>11870647687</v>
+        <v>10732938935</v>
       </c>
       <c r="F654" s="4">
-        <v>5990089529</v>
+        <v>106656990879</v>
       </c>
       <c r="N654" s="1" t="s">
         <v>1655</v>
@@ -24670,17 +24670,17 @@
       </c>
       <c r="C655" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.870516779</v>
+        <v>10.732820685</v>
       </c>
       <c r="D655" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.90054776</v>
+        <v>10.6656958753</v>
       </c>
       <c r="E655" s="4">
-        <v>11870516779</v>
+        <v>10732820685</v>
       </c>
       <c r="F655" s="4">
-        <v>5990054776</v>
+        <v>106656958753</v>
       </c>
       <c r="N655" s="1" t="s">
         <v>1655</v>
@@ -24692,17 +24692,17 @@
       </c>
       <c r="C656" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.870285350</v>
+        <v>10.732611446</v>
       </c>
       <c r="D656" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>59.90061675</v>
+        <v>10.6656964438</v>
       </c>
       <c r="E656" s="4">
-        <v>11870285350</v>
+        <v>10732611446</v>
       </c>
       <c r="F656" s="4">
-        <v>5990061675</v>
+        <v>106656964438</v>
       </c>
       <c r="N656" s="1" t="s">
         <v>1655</v>
@@ -24714,17 +24714,17 @@
       </c>
       <c r="C657" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.876184897</v>
+        <v>10.737903333</v>
       </c>
       <c r="D657" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>60.05495646</v>
+        <v>10.6671090000</v>
       </c>
       <c r="E657" s="4">
-        <v>11876184897</v>
+        <v>10737903333</v>
       </c>
       <c r="F657" s="4">
-        <v>6005495646</v>
+        <v>106671090000</v>
       </c>
       <c r="N657" s="1" t="s">
         <v>1655</v>
@@ -24736,17 +24736,17 @@
       </c>
       <c r="C658" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.876140528</v>
+        <v>10.737863261</v>
       </c>
       <c r="D658" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>60.05480778</v>
+        <v>10.6671076288</v>
       </c>
       <c r="E658" s="4">
-        <v>11876140528</v>
+        <v>10737863261</v>
       </c>
       <c r="F658" s="4">
-        <v>6005480778</v>
+        <v>106671076288</v>
       </c>
       <c r="N658" s="1" t="s">
         <v>1655</v>
@@ -24758,17 +24758,17 @@
       </c>
       <c r="C659" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.876268073</v>
+        <v>10.737977733</v>
       </c>
       <c r="D659" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>60.05788198</v>
+        <v>10.6671357678</v>
       </c>
       <c r="E659" s="4">
-        <v>11876268073</v>
+        <v>10737977733</v>
       </c>
       <c r="F659" s="4">
-        <v>6005788198</v>
+        <v>106671357678</v>
       </c>
       <c r="N659" s="1" t="s">
         <v>1655</v>
@@ -24780,17 +24780,17 @@
       </c>
       <c r="C660" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.876302989</v>
+        <v>10.738008952</v>
       </c>
       <c r="D660" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>60.05916211</v>
+        <v>10.6671474803</v>
       </c>
       <c r="E660" s="4">
-        <v>11876302989</v>
+        <v>10738008952</v>
       </c>
       <c r="F660" s="4">
-        <v>6005916211</v>
+        <v>106671474803</v>
       </c>
       <c r="N660" s="1" t="s">
         <v>1655</v>
@@ -24802,17 +24802,17 @@
       </c>
       <c r="C661" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.876445444</v>
+        <v>10.738136791</v>
       </c>
       <c r="D661" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>60.06265000</v>
+        <v>10.6671794054</v>
       </c>
       <c r="E661" s="4">
-        <v>11876445444</v>
+        <v>10738136791</v>
       </c>
       <c r="F661" s="4">
-        <v>6006265000</v>
+        <v>106671794054</v>
       </c>
       <c r="N661" s="1" t="s">
         <v>1655</v>
@@ -24824,17 +24824,17 @@
       </c>
       <c r="C662" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.876597113</v>
+        <v>10.738272834</v>
       </c>
       <c r="D662" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>60.06660039</v>
+        <v>10.6672155612</v>
       </c>
       <c r="E662" s="4">
-        <v>11876597113</v>
+        <v>10738272834</v>
       </c>
       <c r="F662" s="4">
-        <v>6006660039</v>
+        <v>106672155612</v>
       </c>
       <c r="N662" s="1" t="s">
         <v>1655</v>
@@ -24846,17 +24846,17 @@
       </c>
       <c r="C663" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>11.876766329</v>
+        <v>10.738424635</v>
       </c>
       <c r="D663" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>60.07093534</v>
+        <v>10.6672552374</v>
       </c>
       <c r="E663" s="4">
-        <v>11876766329</v>
+        <v>10738424635</v>
       </c>
       <c r="F663" s="4">
-        <v>6007093534</v>
+        <v>106672552374</v>
       </c>
       <c r="N663" s="1" t="s">
         <v>1655</v>

</xml_diff>